<commit_message>
constraint 1 and 2 ok and clean
</commit_message>
<xml_diff>
--- a/Results/Planning.xlsx
+++ b/Results/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Desktop/Git_SDP/SDP_Optimization/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0616505-F6FF-B243-9672-AE760E3A4A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDFAE97-CDA5-1842-B27C-A3A46C548A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planning_toy_instance" sheetId="1" r:id="rId1"/>
@@ -1821,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView zoomScale="81" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2928,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA2FD1F-E0D1-ED4E-B50F-BF18CBCC44AC}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3863,14 +3863,16 @@
   <dimension ref="A1:FJ117"/>
   <sheetViews>
     <sheetView zoomScale="64" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="3.83203125" style="1" customWidth="1"/>
-    <col min="13" max="22" width="10.83203125" style="1"/>
+    <col min="13" max="17" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="10.83203125" style="1" customWidth="1"/>
+    <col min="19" max="22" width="10.83203125" style="1"/>
     <col min="23" max="23" width="3.83203125" style="1" customWidth="1"/>
     <col min="24" max="33" width="10.83203125" style="1"/>
     <col min="34" max="34" width="3.83203125" style="1" customWidth="1"/>

</xml_diff>